<commit_message>
employee dta temp set
</commit_message>
<xml_diff>
--- a/HRM_SYS/media/emp_temp/employee_template.xlsx
+++ b/HRM_SYS/media/emp_temp/employee_template.xlsx
@@ -616,7 +616,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>koshtech.site@gmail.com</t>
         </is>
       </c>
       <c r="H2" s="2" t="n">
@@ -652,9 +652,15 @@
           <t>None</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
       <c r="R2" t="inlineStr">
         <is>
           <t>None</t>
@@ -666,7 +672,9 @@
       <c r="T2" s="2" t="n">
         <v>45234</v>
       </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
       <c r="V2" t="inlineStr">
         <is>
           <t>None</t>

</xml_diff>